<commit_message>
Paginated and Sorted table
</commit_message>
<xml_diff>
--- a/frontend/research-table/public/research-list.xlsx
+++ b/frontend/research-table/public/research-list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="422">
   <si>
     <t>Achterberg et al. (2018)</t>
   </si>
@@ -122,9 +122,6 @@
     <t>Guieu et al., 2002</t>
   </si>
   <si>
-    <t>Guieu et al., in review 2018</t>
-  </si>
-  <si>
     <t>Strzelec et al. 2020</t>
   </si>
   <si>
@@ -204,9 +201,6 @@
   </si>
   <si>
     <t>Uematsu et al., 2003</t>
-  </si>
-  <si>
-    <t>unknown-Myriokefalitakis(2018)</t>
   </si>
   <si>
     <t>Virkkula et al., 1999</t>
@@ -1034,9 +1028,6 @@
     <t>https://analyticalsciencejournals.onlinelibrary.wiley.com/doi/abs/10.1002/(SICI)1097-4539(199807/08)27:4%3C236::AID-XRS292%3E3.0.CO;2-F?casa_token=dJ8QDVwf4SYAAAAA:wIjrYOfm7Hqy2NQ6mAATPnMe1UEFyifSdtvY1mQXUL22W0qWRwhBOzkOIOemNsX5klhGIXO_AB0LLg</t>
   </si>
   <si>
-    <t>https://doi.org/10.1034/j.1600-0889.1996.t01-1-00011.x</t>
-  </si>
-  <si>
     <t>Multi-elemental composition and sources of the high Arctic atmospheric aerosol during summer and autumn</t>
   </si>
   <si>
@@ -1073,24 +1064,6 @@
     <t>https://doi.org/10.1016/S0168-583X(98)01069-6</t>
   </si>
   <si>
-    <t>Five-year study on the atmospheric aerosol composition, sources and chemical mass closure at two sites in Southern Norway</t>
-  </si>
-  <si>
-    <t>On source apportionment of the fine aerosol : experience at the University of Gent</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1016/S0021-8502(00)90111-3</t>
-  </si>
-  <si>
-    <t>https://www.sciencedirect.com/science/article/abs/pii/S0021850200901113?via%3Dihub</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1016/S0021-8502(00)90187-3</t>
-  </si>
-  <si>
-    <t>https://www.sciencedirect.com/science/article/abs/pii/S0021850200901873?via%3Dihub</t>
-  </si>
-  <si>
     <t>Nuclear microprobe analysis of atmospheric aerosol samples: Comparison with bulk measurements and analyses of individual particles</t>
   </si>
   <si>
@@ -1277,15 +1250,6 @@
     <t>https://www.sciencedirect.com/science/article/pii/S1352231006012702?casa_token=8nyqNSFSEqwAAAAA:UKA5IZGXyJm2dAuElmPCsESubWyAWh8tSDXHLU8w9U1vCTMJuZvBKvKhWmGUH9b5LiqNearAsQ</t>
   </si>
   <si>
-    <t>Aerosol chemical mass closure during the EUROTRAC-2 AEROSOL Intercomparison 2000</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1016/S0168-583X(01)01048-5</t>
-  </si>
-  <si>
-    <t>https://www.sciencedirect.com/science/article/pii/S0168583X01010485?casa_token=pcvnmvH5ANcAAAAA:xh41ZyaCAMixjKW8_rjoOtf-WagjQ09GM-EtrUophE64lsYDPmjNiOhBRQlbt79FSWkrOPTODA</t>
-  </si>
-  <si>
     <t>Two-year study of atmospheric aerosols in Alta Floresta, Brazil: Multielemental composition and source apportionment</t>
   </si>
   <si>
@@ -1329,6 +1293,45 @@
   </si>
   <si>
     <t>https://agupubs.onlinelibrary.wiley.com/doi/10.1029/2003JD003958</t>
+  </si>
+  <si>
+    <t>Maria Kanakidou, Stelios Myriokefalitakis and Kostas Tsigaridis (2018)</t>
+  </si>
+  <si>
+    <t>Guieu et al.</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.3402/tellusb.v48i2.15892</t>
+  </si>
+  <si>
+    <t>Long-term aerosol study in southern Norway, and the relationship of aerosol components to source regions</t>
+  </si>
+  <si>
+    <t>Long-term observations of regional aerosol composition at two sites in Indonesia</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/abs/pii/S0168583X01010540</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/S0168-583X(01)01054-0</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/S0021-8502(00)90755-9</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/abs/pii/S0021850200907559?via%3Dihub</t>
+  </si>
+  <si>
+    <t>Aerosol composition at Jabiru, Australia, and impact of biomass burning</t>
+  </si>
+  <si>
+    <t>Long-term aerosol composition measurements and source apportionment at Rukomechi, Zimbabwe</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/S0021-8502(00)90237-4</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/abs/pii/S0021850200902374?via%3Dihub</t>
   </si>
 </sst>
 </file>
@@ -1714,8 +1717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="B105" sqref="B105"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1725,26 +1728,27 @@
     <col min="3" max="3" width="27.44140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="29.109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="27.5546875" style="2"/>
+    <col min="7" max="7" width="51.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>66</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -1755,13 +1759,13 @@
         <v>2018</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>164</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -1772,13 +1776,13 @@
         <v>2010</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>167</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -1789,13 +1793,13 @@
         <v>1995</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -1806,13 +1810,13 @@
         <v>1996</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>175</v>
-      </c>
       <c r="E5" s="6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -1823,13 +1827,13 @@
         <v>2002</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>415</v>
+        <v>403</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>416</v>
+        <v>404</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -1840,13 +1844,13 @@
         <v>2006</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>184</v>
-      </c>
       <c r="E7" s="6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -1857,13 +1861,13 @@
         <v>2006</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>181</v>
-      </c>
       <c r="E8" s="6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -1874,13 +1878,13 @@
         <v>2006</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>176</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
@@ -1891,13 +1895,13 @@
         <v>2013</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -1908,13 +1912,13 @@
         <v>2017</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -1925,13 +1929,13 @@
         <v>2002</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -1942,13 +1946,13 @@
         <v>1989</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>196</v>
-      </c>
       <c r="E13" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -1959,13 +1963,13 @@
         <v>1992</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>199</v>
-      </c>
       <c r="E14" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
@@ -1976,13 +1980,13 @@
         <v>1992</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>201</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -1993,13 +1997,13 @@
         <v>2012</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
@@ -2010,13 +2014,13 @@
         <v>2009</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>209</v>
-      </c>
       <c r="E17" s="6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
@@ -2027,13 +2031,13 @@
         <v>2006</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="E18" s="6" t="s">
         <v>210</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
@@ -2044,13 +2048,13 @@
         <v>2010</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="E19" s="6" t="s">
         <v>213</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
@@ -2061,13 +2065,13 @@
         <v>2013</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>216</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
@@ -2078,13 +2082,13 @@
         <v>2018</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="E21" s="6" t="s">
         <v>245</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
@@ -2092,22 +2096,22 @@
         <v>20</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>418</v>
+        <v>406</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>419</v>
+        <v>407</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>420</v>
+        <v>408</v>
       </c>
       <c r="G22" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="I22" s="9" t="s">
         <v>248</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>249</v>
-      </c>
-      <c r="I22" s="9" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
@@ -2126,13 +2130,13 @@
         <v>2005</v>
       </c>
       <c r="C24" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="D24" s="6" t="s">
-        <v>253</v>
-      </c>
       <c r="E24" s="6" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
@@ -2143,13 +2147,13 @@
         <v>2004</v>
       </c>
       <c r="C25" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="D25" s="6" t="s">
-        <v>256</v>
-      </c>
       <c r="E25" s="6" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
@@ -2160,13 +2164,13 @@
         <v>1991</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="E26" s="6" t="s">
         <v>257</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>258</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
@@ -2177,11 +2181,11 @@
         <v>1994</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D27" s="7"/>
       <c r="E27" s="6" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
@@ -2192,13 +2196,13 @@
         <v>1993</v>
       </c>
       <c r="C28" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="E28" s="6" t="s">
         <v>262</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
@@ -2209,13 +2213,13 @@
         <v>2007</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="E29" s="6" t="s">
         <v>265</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>266</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="72" x14ac:dyDescent="0.3">
@@ -2226,13 +2230,13 @@
         <v>2013</v>
       </c>
       <c r="C30" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="E30" s="6" t="s">
         <v>268</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>269</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
@@ -2243,13 +2247,13 @@
         <v>2020</v>
       </c>
       <c r="C31" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="E31" s="6" t="s">
         <v>271</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>272</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
@@ -2260,13 +2264,13 @@
         <v>2005</v>
       </c>
       <c r="C32" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="E32" s="6" t="s">
         <v>274</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>275</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="72" x14ac:dyDescent="0.3">
@@ -2277,1217 +2281,1220 @@
         <v>2002</v>
       </c>
       <c r="C33" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="D33" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="D33" s="6" t="s">
-        <v>279</v>
-      </c>
       <c r="E33" s="6" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>32</v>
+        <v>410</v>
       </c>
       <c r="B34">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C34" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="E34" s="6" t="s">
         <v>280</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B35">
         <v>2020</v>
       </c>
       <c r="C35" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="E35" s="6" t="s">
         <v>283</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>284</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B36">
         <v>2021</v>
       </c>
       <c r="C36" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="E36" s="6" t="s">
         <v>286</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B37">
         <v>2016</v>
       </c>
       <c r="C37" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="E37" s="6" t="s">
         <v>289</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>290</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B38">
         <v>1999</v>
       </c>
       <c r="C38" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="E38" s="6" t="s">
         <v>292</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>293</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39">
         <v>2000</v>
       </c>
       <c r="C39" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="E39" s="6" t="s">
         <v>295</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>296</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40">
         <v>2005</v>
       </c>
       <c r="C40" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="E40" s="6" t="s">
         <v>301</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>302</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41">
         <v>2007</v>
       </c>
       <c r="C41" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="E41" s="6" t="s">
         <v>298</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B42">
         <v>1995</v>
       </c>
       <c r="C42" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="E42" s="6" t="s">
         <v>304</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>305</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43">
         <v>2010</v>
       </c>
       <c r="C43" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="E43" s="6" t="s">
         <v>310</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>311</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B44">
         <v>2016</v>
       </c>
       <c r="C44" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="E44" s="6" t="s">
         <v>313</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>314</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45">
         <v>1992</v>
       </c>
       <c r="C45" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="D45" s="6" t="s">
         <v>316</v>
       </c>
-      <c r="D45" s="6" t="s">
-        <v>318</v>
-      </c>
       <c r="E45" s="6" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="144" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B46">
         <v>1998</v>
       </c>
       <c r="C46" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="E46" s="6" t="s">
         <v>319</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>320</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B47">
         <v>1996</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D47" s="6" t="s">
+        <v>411</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="G47" s="5" t="s">
         <v>322</v>
-      </c>
-      <c r="E47" s="6" t="s">
-        <v>324</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B48">
         <v>1997</v>
       </c>
       <c r="C48" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>401</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>402</v>
+      </c>
+      <c r="G48" s="2" t="s">
         <v>412</v>
-      </c>
-      <c r="D48" s="9" t="s">
-        <v>413</v>
-      </c>
-      <c r="E48" s="9" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B49">
         <v>2002</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B50">
         <v>2006</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B51">
         <v>1996</v>
       </c>
       <c r="C51" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="E51" s="6" t="s">
         <v>307</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>308</v>
-      </c>
-      <c r="E51" s="6" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B52">
         <v>1999</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B53">
         <v>1997</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B54">
         <v>2000</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>335</v>
+        <v>418</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>339</v>
+        <v>416</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>340</v>
+        <v>417</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B55">
         <v>2007</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B56">
         <v>2000</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>336</v>
+        <v>419</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>337</v>
+        <v>420</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>338</v>
+        <v>421</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B57">
         <v>2003</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B58">
         <v>2001</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>409</v>
+        <v>397</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>411</v>
+        <v>399</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B59">
         <v>2002</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>403</v>
+        <v>413</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>404</v>
+        <v>415</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>405</v>
+        <v>414</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B60">
         <v>2002</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>406</v>
+        <v>394</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>407</v>
+        <v>395</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>408</v>
+        <v>396</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B61">
         <v>2007</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>400</v>
+        <v>391</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>402</v>
+        <v>393</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B62">
         <v>2003</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>398</v>
+        <v>389</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>399</v>
+        <v>390</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B63">
         <v>2015</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B64">
         <v>1989</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>391</v>
+        <v>382</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B65">
         <v>1969</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>388</v>
+        <v>379</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>389</v>
+        <v>380</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B66">
         <v>1986</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>387</v>
+        <v>378</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B67">
         <v>1999</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B68">
         <v>1979</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B69">
         <v>2018</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B70">
         <v>2012</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B71">
         <v>2011</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B72">
         <v>1985</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B73">
         <v>2003</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
-        <v>60</v>
+        <v>409</v>
       </c>
       <c r="B74">
         <v>2018</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B75">
         <v>1999</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B76">
         <v>2008</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="B77">
         <v>2008</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B78">
         <v>2006</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="E78" s="6" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D81" s="6" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D84" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D85" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D90" s="6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -3605,69 +3612,64 @@
     <hyperlink ref="D45" r:id="rId111"/>
     <hyperlink ref="D46" r:id="rId112"/>
     <hyperlink ref="E46" r:id="rId113"/>
-    <hyperlink ref="D47" r:id="rId114"/>
-    <hyperlink ref="E47" r:id="rId115"/>
-    <hyperlink ref="G47" r:id="rId116"/>
-    <hyperlink ref="D49" r:id="rId117"/>
-    <hyperlink ref="E49" r:id="rId118"/>
-    <hyperlink ref="D50" r:id="rId119"/>
-    <hyperlink ref="E50" r:id="rId120"/>
-    <hyperlink ref="E52" r:id="rId121"/>
-    <hyperlink ref="D52" r:id="rId122"/>
-    <hyperlink ref="D56" r:id="rId123" tooltip="Persistent link using digital object identifier"/>
-    <hyperlink ref="D54" r:id="rId124" tooltip="Persistent link using digital object identifier"/>
-    <hyperlink ref="E53" r:id="rId125"/>
-    <hyperlink ref="D53" r:id="rId126"/>
-    <hyperlink ref="D55" r:id="rId127"/>
-    <hyperlink ref="E55" r:id="rId128"/>
-    <hyperlink ref="E57" r:id="rId129"/>
-    <hyperlink ref="D78" r:id="rId130"/>
-    <hyperlink ref="E78" r:id="rId131"/>
-    <hyperlink ref="D76" r:id="rId132"/>
-    <hyperlink ref="E76" r:id="rId133"/>
-    <hyperlink ref="E77" r:id="rId134"/>
-    <hyperlink ref="D75" r:id="rId135"/>
-    <hyperlink ref="E75" r:id="rId136"/>
-    <hyperlink ref="D74" r:id="rId137"/>
-    <hyperlink ref="E74" r:id="rId138"/>
-    <hyperlink ref="E73" r:id="rId139"/>
-    <hyperlink ref="D73" r:id="rId140"/>
-    <hyperlink ref="E72" r:id="rId141"/>
-    <hyperlink ref="D72" r:id="rId142"/>
-    <hyperlink ref="D71" r:id="rId143"/>
-    <hyperlink ref="E71" r:id="rId144"/>
-    <hyperlink ref="D70" r:id="rId145"/>
-    <hyperlink ref="E70" r:id="rId146"/>
-    <hyperlink ref="D69" r:id="rId147"/>
-    <hyperlink ref="E69" r:id="rId148"/>
-    <hyperlink ref="D68" r:id="rId149"/>
-    <hyperlink ref="E68" r:id="rId150"/>
-    <hyperlink ref="E67" r:id="rId151"/>
-    <hyperlink ref="D67" r:id="rId152"/>
-    <hyperlink ref="E66" r:id="rId153"/>
-    <hyperlink ref="D66" r:id="rId154"/>
-    <hyperlink ref="D65" r:id="rId155"/>
-    <hyperlink ref="E65" r:id="rId156"/>
-    <hyperlink ref="E64" r:id="rId157"/>
-    <hyperlink ref="D64" r:id="rId158"/>
-    <hyperlink ref="D63" r:id="rId159"/>
-    <hyperlink ref="E63" r:id="rId160"/>
-    <hyperlink ref="D62" r:id="rId161"/>
-    <hyperlink ref="E62" r:id="rId162"/>
-    <hyperlink ref="D61" r:id="rId163"/>
-    <hyperlink ref="E61" r:id="rId164"/>
-    <hyperlink ref="D59" r:id="rId165"/>
-    <hyperlink ref="E59" r:id="rId166"/>
-    <hyperlink ref="D60" r:id="rId167"/>
-    <hyperlink ref="E60" r:id="rId168"/>
-    <hyperlink ref="E58" r:id="rId169"/>
-    <hyperlink ref="D58" r:id="rId170"/>
-    <hyperlink ref="D48" r:id="rId171"/>
-    <hyperlink ref="E48" r:id="rId172"/>
-    <hyperlink ref="D6" r:id="rId173"/>
-    <hyperlink ref="E6" r:id="rId174"/>
+    <hyperlink ref="E47" r:id="rId114"/>
+    <hyperlink ref="G47" r:id="rId115"/>
+    <hyperlink ref="D49" r:id="rId116"/>
+    <hyperlink ref="E49" r:id="rId117"/>
+    <hyperlink ref="D50" r:id="rId118"/>
+    <hyperlink ref="E50" r:id="rId119"/>
+    <hyperlink ref="E52" r:id="rId120"/>
+    <hyperlink ref="D52" r:id="rId121"/>
+    <hyperlink ref="E53" r:id="rId122"/>
+    <hyperlink ref="D53" r:id="rId123"/>
+    <hyperlink ref="D55" r:id="rId124"/>
+    <hyperlink ref="E55" r:id="rId125"/>
+    <hyperlink ref="E57" r:id="rId126"/>
+    <hyperlink ref="D78" r:id="rId127"/>
+    <hyperlink ref="E78" r:id="rId128"/>
+    <hyperlink ref="D76" r:id="rId129"/>
+    <hyperlink ref="E76" r:id="rId130"/>
+    <hyperlink ref="E77" r:id="rId131"/>
+    <hyperlink ref="D75" r:id="rId132"/>
+    <hyperlink ref="E75" r:id="rId133"/>
+    <hyperlink ref="D74" r:id="rId134"/>
+    <hyperlink ref="E74" r:id="rId135"/>
+    <hyperlink ref="E73" r:id="rId136"/>
+    <hyperlink ref="D73" r:id="rId137"/>
+    <hyperlink ref="E72" r:id="rId138"/>
+    <hyperlink ref="D72" r:id="rId139"/>
+    <hyperlink ref="D71" r:id="rId140"/>
+    <hyperlink ref="E71" r:id="rId141"/>
+    <hyperlink ref="D70" r:id="rId142"/>
+    <hyperlink ref="E70" r:id="rId143"/>
+    <hyperlink ref="D69" r:id="rId144"/>
+    <hyperlink ref="E69" r:id="rId145"/>
+    <hyperlink ref="D68" r:id="rId146"/>
+    <hyperlink ref="E68" r:id="rId147"/>
+    <hyperlink ref="E67" r:id="rId148"/>
+    <hyperlink ref="D67" r:id="rId149"/>
+    <hyperlink ref="E66" r:id="rId150"/>
+    <hyperlink ref="D66" r:id="rId151"/>
+    <hyperlink ref="D65" r:id="rId152"/>
+    <hyperlink ref="E65" r:id="rId153"/>
+    <hyperlink ref="E64" r:id="rId154"/>
+    <hyperlink ref="D64" r:id="rId155"/>
+    <hyperlink ref="D63" r:id="rId156"/>
+    <hyperlink ref="E63" r:id="rId157"/>
+    <hyperlink ref="D62" r:id="rId158"/>
+    <hyperlink ref="E62" r:id="rId159"/>
+    <hyperlink ref="D61" r:id="rId160"/>
+    <hyperlink ref="E61" r:id="rId161"/>
+    <hyperlink ref="D60" r:id="rId162"/>
+    <hyperlink ref="E60" r:id="rId163"/>
+    <hyperlink ref="E58" r:id="rId164"/>
+    <hyperlink ref="D58" r:id="rId165"/>
+    <hyperlink ref="D48" r:id="rId166"/>
+    <hyperlink ref="E48" r:id="rId167"/>
+    <hyperlink ref="D6" r:id="rId168"/>
+    <hyperlink ref="E6" r:id="rId169"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId175"/>
+  <pageSetup orientation="portrait" r:id="rId170"/>
 </worksheet>
 </file>
</xml_diff>